<commit_message>
Updated About Page with new Application Icon
Needed icon for SourceForge.  Figured might as well update app and all templates too.  Incremented build number too.
</commit_message>
<xml_diff>
--- a/samples/mtcm_sample_1.xlsx
+++ b/samples/mtcm_sample_1.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC557886-9321-44F5-AEBA-2033266866BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F316A412-5DD4-4B3C-A45A-1A87692B2B51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25116" yWindow="1368" windowWidth="12984" windowHeight="10212" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="36" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="34" r:id="rId2"/>
     <sheet name="Test Run Log" sheetId="35" r:id="rId3"/>
     <sheet name="Report" sheetId="1" r:id="rId4"/>
-    <sheet name="About" sheetId="38" r:id="rId5"/>
+    <sheet name="About" sheetId="39" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Cases'!$B$18:$E$319</definedName>
@@ -650,13 +650,13 @@
     <t>▪</t>
   </si>
   <si>
-    <t xml:space="preserve"> v5.01.44289</t>
-  </si>
-  <si>
     <t>Day #3 Testing</t>
   </si>
   <si>
     <t>Day #4 Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> v5.01.44294</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1436,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="32" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1728,9 +1728,6 @@
     <xf numFmtId="0" fontId="30" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1745,6 +1742,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="33" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1766,14 +1769,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1790,17 +1793,14 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1808,8 +1808,11 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -9194,23 +9197,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3036024</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>514896</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFBB2022-CA7A-4806-AA4F-0D581BB3BEBC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16119A88-4E83-4911-966B-B82380E3F6A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9233,7 +9236,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="4041864" y="60960"/>
           <a:ext cx="1223556" cy="853440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9257,13 +9260,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>112644</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>338051</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>40871</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>33132</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -9271,7 +9274,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D60F16D1-D1BE-4376-9662-CCFAFD057AB8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20A53405-43F6-4675-865E-BA2C221357D0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9294,7 +9297,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="112644" y="2491742"/>
+          <a:off x="112644" y="2446022"/>
           <a:ext cx="934067" cy="947530"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9316,16 +9319,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>514844</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>3975</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>217665</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2948939</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>178905</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -9333,7 +9336,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97F321C4-7663-45F4-A3D6-A344C833B290}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D368F32-6B28-46FE-AEB4-6093E2F05EC2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9341,8 +9344,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1223504" y="2495715"/>
-          <a:ext cx="2959875" cy="529425"/>
+          <a:off x="1223505" y="2446020"/>
+          <a:ext cx="2952255" cy="529425"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
@@ -9439,6 +9442,67 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>253746</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CA56A91-4B84-4B27-A077-F99C1EAA56DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="962406" cy="937260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -9788,10 +9852,10 @@
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="59"/>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="128"/>
+      <c r="C2" s="129"/>
       <c r="D2" s="59"/>
     </row>
     <row r="3" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -9861,7 +9925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EC35F8-1315-4AD0-BB4E-D826F75C5B55}">
   <dimension ref="A1:L320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -9903,13 +9967,13 @@
       <c r="D2" s="64"/>
       <c r="E2" s="64"/>
       <c r="F2" s="119"/>
-      <c r="G2" s="129" t="s">
+      <c r="G2" s="130" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="130"/>
-      <c r="K2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="132"/>
       <c r="L2" s="4"/>
     </row>
     <row r="3" spans="1:12" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -10186,12 +10250,12 @@
       <c r="A17" s="119" t="s">
         <v>135</v>
       </c>
-      <c r="B17" s="129" t="s">
+      <c r="B17" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="130"/>
-      <c r="D17" s="130"/>
-      <c r="E17" s="131"/>
+      <c r="C17" s="131"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="132"/>
       <c r="F17" s="119" t="s">
         <v>135</v>
       </c>
@@ -14140,41 +14204,41 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
-      <c r="B3" s="132" t="s">
+      <c r="B3" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="133" t="s">
+      <c r="C3" s="134" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="134" t="s">
+      <c r="D3" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="132" t="s">
+      <c r="E3" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="134" t="s">
+      <c r="F3" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
-      <c r="K3" s="134"/>
-      <c r="L3" s="134" t="s">
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="134"/>
-      <c r="N3" s="134"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="134"/>
+      <c r="M3" s="135"/>
+      <c r="N3" s="135"/>
+      <c r="O3" s="135"/>
+      <c r="P3" s="135"/>
       <c r="Q3" s="13"/>
     </row>
     <row r="4" spans="1:17" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
-      <c r="B4" s="132"/>
-      <c r="C4" s="133"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="132"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="134"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="133"/>
       <c r="F4" s="35" t="s">
         <v>18</v>
       </c>
@@ -14318,7 +14382,7 @@
         <v>98</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D7" s="17">
         <v>44283</v>
@@ -14367,7 +14431,7 @@
         <v>130</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D8" s="17">
         <v>44284</v>
@@ -14491,44 +14555,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" s="93" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="B1" s="137" t="s">
+      <c r="B1" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
-      <c r="L1" s="137"/>
-      <c r="M1" s="137"/>
-      <c r="N1" s="137"/>
-      <c r="O1" s="137"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="146"/>
+      <c r="O1" s="146"/>
       <c r="Q1" s="94"/>
     </row>
     <row r="2" spans="2:17" s="57" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C2" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="136" t="str">
+      <c r="D2" s="145" t="str">
         <f>IF(Properties!$C$4=0, "", Properties!$C$4)</f>
         <v>Data Research Labs</v>
       </c>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
       <c r="M2" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="135" t="str" cm="1">
+      <c r="N2" s="144" t="str" cm="1">
         <f t="array" ref="N2">INDEX('Test Run Log'!$B$5:$B$8,MATCH(MAX(COUNTIF('Test Run Log'!$B$5:$B$8, "&lt;" &amp; 'Test Run Log'!$B$5:$B$8)), COUNTIF('Test Run Log'!$B$5:$B$8, "&lt;"&amp;'Test Run Log'!$B$5:$B$8),0))</f>
         <v>R4</v>
       </c>
-      <c r="O2" s="135"/>
+      <c r="O2" s="144"/>
       <c r="Q2" s="95"/>
     </row>
     <row r="3" spans="2:17" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -14536,22 +14600,22 @@
       <c r="C3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="135" t="str">
+      <c r="D3" s="144" t="str">
         <f>IF(Properties!$C$6=0, "", Properties!$C$6)</f>
         <v>My Test Case Manager (self-test)</v>
       </c>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
       <c r="M3" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="N3" s="135" t="str">
+      <c r="N3" s="144" t="str">
         <f>IF(Properties!$C$8=0, "", Properties!$C$8)</f>
         <v>Matt Pierce</v>
       </c>
-      <c r="O3" s="135"/>
+      <c r="O3" s="144"/>
       <c r="Q3" s="95"/>
     </row>
     <row r="4" spans="2:17" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -14561,11 +14625,11 @@
       <c r="M4" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="136">
+      <c r="N4" s="145">
         <f>SUM(C14:G14)</f>
         <v>74</v>
       </c>
-      <c r="O4" s="136"/>
+      <c r="O4" s="145"/>
       <c r="Q4" s="95"/>
     </row>
     <row r="5" spans="2:17" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -14575,34 +14639,34 @@
       <c r="M5" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="N5" s="136">
+      <c r="N5" s="145">
         <f>SUM(K14:M14)</f>
         <v>14</v>
       </c>
-      <c r="O5" s="136"/>
+      <c r="O5" s="145"/>
       <c r="Q5" s="95"/>
     </row>
     <row r="6" spans="2:17" ht="6.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:17" s="54" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="138" t="str">
+      <c r="B7" s="139" t="str">
         <f xml:space="preserve"> "TEST CASE COUNTS - SNAPSHOT @ " &amp; $N$2</f>
         <v>TEST CASE COUNTS - SNAPSHOT @ R4</v>
       </c>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="139"/>
-      <c r="F7" s="139"/>
-      <c r="G7" s="139"/>
-      <c r="H7" s="140"/>
-      <c r="J7" s="138" t="str">
+      <c r="C7" s="140"/>
+      <c r="D7" s="140"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="140"/>
+      <c r="G7" s="140"/>
+      <c r="H7" s="141"/>
+      <c r="J7" s="139" t="str">
         <f xml:space="preserve"> "DEFECTS - SNAPSHOT @ " &amp; $N$2</f>
         <v>DEFECTS - SNAPSHOT @ R4</v>
       </c>
-      <c r="K7" s="139"/>
-      <c r="L7" s="139"/>
-      <c r="M7" s="139"/>
-      <c r="N7" s="139"/>
-      <c r="O7" s="140"/>
+      <c r="K7" s="140"/>
+      <c r="L7" s="140"/>
+      <c r="M7" s="140"/>
+      <c r="N7" s="140"/>
+      <c r="O7" s="141"/>
       <c r="Q7" s="55"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
@@ -14779,49 +14843,49 @@
       <c r="Q16" s="55"/>
     </row>
     <row r="17" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="138" t="str">
+      <c r="B17" s="139" t="str">
         <f xml:space="preserve"> "TEST CASE COUNTS - TREND"</f>
         <v>TEST CASE COUNTS - TREND</v>
       </c>
-      <c r="C17" s="139"/>
-      <c r="D17" s="139"/>
-      <c r="E17" s="139"/>
-      <c r="F17" s="139"/>
-      <c r="G17" s="139"/>
-      <c r="H17" s="140"/>
-      <c r="J17" s="138" t="str">
+      <c r="C17" s="140"/>
+      <c r="D17" s="140"/>
+      <c r="E17" s="140"/>
+      <c r="F17" s="140"/>
+      <c r="G17" s="140"/>
+      <c r="H17" s="141"/>
+      <c r="J17" s="139" t="str">
         <f xml:space="preserve"> "DEFECTS - TREND"</f>
         <v>DEFECTS - TREND</v>
       </c>
-      <c r="K17" s="139"/>
-      <c r="L17" s="139"/>
-      <c r="M17" s="139"/>
-      <c r="N17" s="139"/>
-      <c r="O17" s="140"/>
+      <c r="K17" s="140"/>
+      <c r="L17" s="140"/>
+      <c r="M17" s="140"/>
+      <c r="N17" s="140"/>
+      <c r="O17" s="141"/>
     </row>
     <row r="28" spans="2:17" s="54" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Q28" s="55"/>
     </row>
     <row r="29" spans="2:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B29" s="138" t="str">
+      <c r="B29" s="139" t="str">
         <f xml:space="preserve"> "TEST CASE EXEC TIME - TREND"</f>
         <v>TEST CASE EXEC TIME - TREND</v>
       </c>
-      <c r="C29" s="139"/>
-      <c r="D29" s="139"/>
-      <c r="E29" s="139"/>
-      <c r="F29" s="139"/>
-      <c r="G29" s="139"/>
-      <c r="H29" s="140"/>
-      <c r="J29" s="138" t="str">
+      <c r="C29" s="140"/>
+      <c r="D29" s="140"/>
+      <c r="E29" s="140"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="141"/>
+      <c r="J29" s="139" t="str">
         <f xml:space="preserve"> "DEFECTS - RELEASABILITY"</f>
         <v>DEFECTS - RELEASABILITY</v>
       </c>
-      <c r="K29" s="139"/>
-      <c r="L29" s="139"/>
-      <c r="M29" s="139"/>
-      <c r="N29" s="139"/>
-      <c r="O29" s="140"/>
+      <c r="K29" s="140"/>
+      <c r="L29" s="140"/>
+      <c r="M29" s="140"/>
+      <c r="N29" s="140"/>
+      <c r="O29" s="141"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="54"/>
@@ -14954,254 +15018,254 @@
     </row>
     <row r="41" spans="1:17" ht="6.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B42" s="138" t="s">
+      <c r="B42" s="139" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="139"/>
-      <c r="D42" s="139"/>
-      <c r="E42" s="139"/>
-      <c r="F42" s="139"/>
-      <c r="G42" s="139"/>
-      <c r="H42" s="139"/>
-      <c r="I42" s="139"/>
-      <c r="J42" s="139"/>
-      <c r="K42" s="139"/>
-      <c r="L42" s="139"/>
-      <c r="M42" s="139"/>
-      <c r="N42" s="139"/>
-      <c r="O42" s="140"/>
+      <c r="C42" s="140"/>
+      <c r="D42" s="140"/>
+      <c r="E42" s="140"/>
+      <c r="F42" s="140"/>
+      <c r="G42" s="140"/>
+      <c r="H42" s="140"/>
+      <c r="I42" s="140"/>
+      <c r="J42" s="140"/>
+      <c r="K42" s="140"/>
+      <c r="L42" s="140"/>
+      <c r="M42" s="140"/>
+      <c r="N42" s="140"/>
+      <c r="O42" s="141"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B43" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="142" t="s">
+      <c r="C43" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="142"/>
-      <c r="E43" s="142"/>
-      <c r="F43" s="142"/>
-      <c r="G43" s="142"/>
-      <c r="H43" s="142"/>
-      <c r="I43" s="142"/>
-      <c r="J43" s="142"/>
-      <c r="K43" s="142"/>
-      <c r="L43" s="142"/>
-      <c r="M43" s="142"/>
-      <c r="N43" s="142"/>
-      <c r="O43" s="142"/>
+      <c r="D43" s="143"/>
+      <c r="E43" s="143"/>
+      <c r="F43" s="143"/>
+      <c r="G43" s="143"/>
+      <c r="H43" s="143"/>
+      <c r="I43" s="143"/>
+      <c r="J43" s="143"/>
+      <c r="K43" s="143"/>
+      <c r="L43" s="143"/>
+      <c r="M43" s="143"/>
+      <c r="N43" s="143"/>
+      <c r="O43" s="143"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B44" s="116"/>
-      <c r="C44" s="143"/>
-      <c r="D44" s="144"/>
-      <c r="E44" s="144"/>
-      <c r="F44" s="144"/>
-      <c r="G44" s="144"/>
-      <c r="H44" s="144"/>
-      <c r="I44" s="144"/>
-      <c r="J44" s="144"/>
-      <c r="K44" s="144"/>
-      <c r="L44" s="144"/>
-      <c r="M44" s="144"/>
-      <c r="N44" s="144"/>
-      <c r="O44" s="145"/>
+      <c r="C44" s="136"/>
+      <c r="D44" s="137"/>
+      <c r="E44" s="137"/>
+      <c r="F44" s="137"/>
+      <c r="G44" s="137"/>
+      <c r="H44" s="137"/>
+      <c r="I44" s="137"/>
+      <c r="J44" s="137"/>
+      <c r="K44" s="137"/>
+      <c r="L44" s="137"/>
+      <c r="M44" s="137"/>
+      <c r="N44" s="137"/>
+      <c r="O44" s="138"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B45" s="116"/>
-      <c r="C45" s="143"/>
-      <c r="D45" s="144"/>
-      <c r="E45" s="144"/>
-      <c r="F45" s="144"/>
-      <c r="G45" s="144"/>
-      <c r="H45" s="144"/>
-      <c r="I45" s="144"/>
-      <c r="J45" s="144"/>
-      <c r="K45" s="144"/>
-      <c r="L45" s="144"/>
-      <c r="M45" s="144"/>
-      <c r="N45" s="144"/>
-      <c r="O45" s="145"/>
+      <c r="C45" s="136"/>
+      <c r="D45" s="137"/>
+      <c r="E45" s="137"/>
+      <c r="F45" s="137"/>
+      <c r="G45" s="137"/>
+      <c r="H45" s="137"/>
+      <c r="I45" s="137"/>
+      <c r="J45" s="137"/>
+      <c r="K45" s="137"/>
+      <c r="L45" s="137"/>
+      <c r="M45" s="137"/>
+      <c r="N45" s="137"/>
+      <c r="O45" s="138"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B46" s="116"/>
-      <c r="C46" s="143"/>
-      <c r="D46" s="144"/>
-      <c r="E46" s="144"/>
-      <c r="F46" s="144"/>
-      <c r="G46" s="144"/>
-      <c r="H46" s="144"/>
-      <c r="I46" s="144"/>
-      <c r="J46" s="144"/>
-      <c r="K46" s="144"/>
-      <c r="L46" s="144"/>
-      <c r="M46" s="144"/>
-      <c r="N46" s="144"/>
-      <c r="O46" s="145"/>
+      <c r="C46" s="136"/>
+      <c r="D46" s="137"/>
+      <c r="E46" s="137"/>
+      <c r="F46" s="137"/>
+      <c r="G46" s="137"/>
+      <c r="H46" s="137"/>
+      <c r="I46" s="137"/>
+      <c r="J46" s="137"/>
+      <c r="K46" s="137"/>
+      <c r="L46" s="137"/>
+      <c r="M46" s="137"/>
+      <c r="N46" s="137"/>
+      <c r="O46" s="138"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="118"/>
-      <c r="C47" s="143"/>
-      <c r="D47" s="144"/>
-      <c r="E47" s="144"/>
-      <c r="F47" s="144"/>
-      <c r="G47" s="144"/>
-      <c r="H47" s="144"/>
-      <c r="I47" s="144"/>
-      <c r="J47" s="144"/>
-      <c r="K47" s="144"/>
-      <c r="L47" s="144"/>
-      <c r="M47" s="144"/>
-      <c r="N47" s="144"/>
-      <c r="O47" s="145"/>
+      <c r="C47" s="136"/>
+      <c r="D47" s="137"/>
+      <c r="E47" s="137"/>
+      <c r="F47" s="137"/>
+      <c r="G47" s="137"/>
+      <c r="H47" s="137"/>
+      <c r="I47" s="137"/>
+      <c r="J47" s="137"/>
+      <c r="K47" s="137"/>
+      <c r="L47" s="137"/>
+      <c r="M47" s="137"/>
+      <c r="N47" s="137"/>
+      <c r="O47" s="138"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
       <c r="B48" s="117"/>
-      <c r="C48" s="143"/>
-      <c r="D48" s="144"/>
-      <c r="E48" s="144"/>
-      <c r="F48" s="144"/>
-      <c r="G48" s="144"/>
-      <c r="H48" s="144"/>
-      <c r="I48" s="144"/>
-      <c r="J48" s="144"/>
-      <c r="K48" s="144"/>
-      <c r="L48" s="144"/>
-      <c r="M48" s="144"/>
-      <c r="N48" s="144"/>
-      <c r="O48" s="145"/>
+      <c r="C48" s="136"/>
+      <c r="D48" s="137"/>
+      <c r="E48" s="137"/>
+      <c r="F48" s="137"/>
+      <c r="G48" s="137"/>
+      <c r="H48" s="137"/>
+      <c r="I48" s="137"/>
+      <c r="J48" s="137"/>
+      <c r="K48" s="137"/>
+      <c r="L48" s="137"/>
+      <c r="M48" s="137"/>
+      <c r="N48" s="137"/>
+      <c r="O48" s="138"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:17" s="54" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B50" s="138" t="s">
+      <c r="B50" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="139"/>
-      <c r="D50" s="139"/>
-      <c r="E50" s="139"/>
-      <c r="F50" s="139"/>
-      <c r="G50" s="139"/>
-      <c r="H50" s="139"/>
-      <c r="I50" s="139"/>
-      <c r="J50" s="139"/>
-      <c r="K50" s="139"/>
-      <c r="L50" s="139"/>
-      <c r="M50" s="139"/>
-      <c r="N50" s="139"/>
-      <c r="O50" s="140"/>
+      <c r="C50" s="140"/>
+      <c r="D50" s="140"/>
+      <c r="E50" s="140"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="140"/>
+      <c r="H50" s="140"/>
+      <c r="I50" s="140"/>
+      <c r="J50" s="140"/>
+      <c r="K50" s="140"/>
+      <c r="L50" s="140"/>
+      <c r="M50" s="140"/>
+      <c r="N50" s="140"/>
+      <c r="O50" s="141"/>
       <c r="Q50" s="55"/>
     </row>
     <row r="51" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="141" t="s">
+      <c r="C51" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="D51" s="141"/>
-      <c r="E51" s="141"/>
-      <c r="F51" s="141"/>
-      <c r="G51" s="141"/>
-      <c r="H51" s="141"/>
-      <c r="I51" s="141"/>
-      <c r="J51" s="141"/>
-      <c r="K51" s="141"/>
-      <c r="L51" s="141"/>
-      <c r="M51" s="141"/>
-      <c r="N51" s="141"/>
-      <c r="O51" s="141"/>
+      <c r="D51" s="142"/>
+      <c r="E51" s="142"/>
+      <c r="F51" s="142"/>
+      <c r="G51" s="142"/>
+      <c r="H51" s="142"/>
+      <c r="I51" s="142"/>
+      <c r="J51" s="142"/>
+      <c r="K51" s="142"/>
+      <c r="L51" s="142"/>
+      <c r="M51" s="142"/>
+      <c r="N51" s="142"/>
+      <c r="O51" s="142"/>
       <c r="Q51" s="55"/>
     </row>
     <row r="52" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52" s="116"/>
-      <c r="C52" s="143"/>
-      <c r="D52" s="144"/>
-      <c r="E52" s="144"/>
-      <c r="F52" s="144"/>
-      <c r="G52" s="144"/>
-      <c r="H52" s="144"/>
-      <c r="I52" s="144"/>
-      <c r="J52" s="144"/>
-      <c r="K52" s="144"/>
-      <c r="L52" s="144"/>
-      <c r="M52" s="144"/>
-      <c r="N52" s="144"/>
-      <c r="O52" s="145"/>
+      <c r="C52" s="136"/>
+      <c r="D52" s="137"/>
+      <c r="E52" s="137"/>
+      <c r="F52" s="137"/>
+      <c r="G52" s="137"/>
+      <c r="H52" s="137"/>
+      <c r="I52" s="137"/>
+      <c r="J52" s="137"/>
+      <c r="K52" s="137"/>
+      <c r="L52" s="137"/>
+      <c r="M52" s="137"/>
+      <c r="N52" s="137"/>
+      <c r="O52" s="138"/>
       <c r="Q52" s="55"/>
     </row>
     <row r="53" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B53" s="116"/>
-      <c r="C53" s="143"/>
-      <c r="D53" s="144"/>
-      <c r="E53" s="144"/>
-      <c r="F53" s="144"/>
-      <c r="G53" s="144"/>
-      <c r="H53" s="144"/>
-      <c r="I53" s="144"/>
-      <c r="J53" s="144"/>
-      <c r="K53" s="144"/>
-      <c r="L53" s="144"/>
-      <c r="M53" s="144"/>
-      <c r="N53" s="144"/>
-      <c r="O53" s="145"/>
+      <c r="C53" s="136"/>
+      <c r="D53" s="137"/>
+      <c r="E53" s="137"/>
+      <c r="F53" s="137"/>
+      <c r="G53" s="137"/>
+      <c r="H53" s="137"/>
+      <c r="I53" s="137"/>
+      <c r="J53" s="137"/>
+      <c r="K53" s="137"/>
+      <c r="L53" s="137"/>
+      <c r="M53" s="137"/>
+      <c r="N53" s="137"/>
+      <c r="O53" s="138"/>
       <c r="Q53" s="55"/>
     </row>
     <row r="54" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="116"/>
-      <c r="C54" s="143"/>
-      <c r="D54" s="144"/>
-      <c r="E54" s="144"/>
-      <c r="F54" s="144"/>
-      <c r="G54" s="144"/>
-      <c r="H54" s="144"/>
-      <c r="I54" s="144"/>
-      <c r="J54" s="144"/>
-      <c r="K54" s="144"/>
-      <c r="L54" s="144"/>
-      <c r="M54" s="144"/>
-      <c r="N54" s="144"/>
-      <c r="O54" s="145"/>
+      <c r="C54" s="136"/>
+      <c r="D54" s="137"/>
+      <c r="E54" s="137"/>
+      <c r="F54" s="137"/>
+      <c r="G54" s="137"/>
+      <c r="H54" s="137"/>
+      <c r="I54" s="137"/>
+      <c r="J54" s="137"/>
+      <c r="K54" s="137"/>
+      <c r="L54" s="137"/>
+      <c r="M54" s="137"/>
+      <c r="N54" s="137"/>
+      <c r="O54" s="138"/>
       <c r="Q54" s="55"/>
     </row>
     <row r="55" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="118"/>
-      <c r="C55" s="143"/>
-      <c r="D55" s="144"/>
-      <c r="E55" s="144"/>
-      <c r="F55" s="144"/>
-      <c r="G55" s="144"/>
-      <c r="H55" s="144"/>
-      <c r="I55" s="144"/>
-      <c r="J55" s="144"/>
-      <c r="K55" s="144"/>
-      <c r="L55" s="144"/>
-      <c r="M55" s="144"/>
-      <c r="N55" s="144"/>
-      <c r="O55" s="145"/>
+      <c r="C55" s="136"/>
+      <c r="D55" s="137"/>
+      <c r="E55" s="137"/>
+      <c r="F55" s="137"/>
+      <c r="G55" s="137"/>
+      <c r="H55" s="137"/>
+      <c r="I55" s="137"/>
+      <c r="J55" s="137"/>
+      <c r="K55" s="137"/>
+      <c r="L55" s="137"/>
+      <c r="M55" s="137"/>
+      <c r="N55" s="137"/>
+      <c r="O55" s="138"/>
       <c r="Q55" s="55"/>
     </row>
     <row r="56" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10"/>
       <c r="B56" s="117"/>
-      <c r="C56" s="143"/>
-      <c r="D56" s="144"/>
-      <c r="E56" s="144"/>
-      <c r="F56" s="144"/>
-      <c r="G56" s="144"/>
-      <c r="H56" s="144"/>
-      <c r="I56" s="144"/>
-      <c r="J56" s="144"/>
-      <c r="K56" s="144"/>
-      <c r="L56" s="144"/>
-      <c r="M56" s="144"/>
-      <c r="N56" s="144"/>
-      <c r="O56" s="145"/>
+      <c r="C56" s="136"/>
+      <c r="D56" s="137"/>
+      <c r="E56" s="137"/>
+      <c r="F56" s="137"/>
+      <c r="G56" s="137"/>
+      <c r="H56" s="137"/>
+      <c r="I56" s="137"/>
+      <c r="J56" s="137"/>
+      <c r="K56" s="137"/>
+      <c r="L56" s="137"/>
+      <c r="M56" s="137"/>
+      <c r="N56" s="137"/>
+      <c r="O56" s="138"/>
       <c r="Q56" s="55"/>
     </row>
     <row r="57" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
@@ -15210,130 +15274,130 @@
       <c r="Q57" s="55"/>
     </row>
     <row r="58" spans="1:17" s="54" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B58" s="138" t="s">
+      <c r="B58" s="139" t="s">
         <v>42</v>
       </c>
-      <c r="C58" s="139"/>
-      <c r="D58" s="139"/>
-      <c r="E58" s="139"/>
-      <c r="F58" s="139"/>
-      <c r="G58" s="139"/>
-      <c r="H58" s="139"/>
-      <c r="I58" s="139"/>
-      <c r="J58" s="139"/>
-      <c r="K58" s="139"/>
-      <c r="L58" s="139"/>
-      <c r="M58" s="139"/>
-      <c r="N58" s="139"/>
-      <c r="O58" s="140"/>
+      <c r="C58" s="140"/>
+      <c r="D58" s="140"/>
+      <c r="E58" s="140"/>
+      <c r="F58" s="140"/>
+      <c r="G58" s="140"/>
+      <c r="H58" s="140"/>
+      <c r="I58" s="140"/>
+      <c r="J58" s="140"/>
+      <c r="K58" s="140"/>
+      <c r="L58" s="140"/>
+      <c r="M58" s="140"/>
+      <c r="N58" s="140"/>
+      <c r="O58" s="141"/>
       <c r="Q58" s="55"/>
     </row>
     <row r="59" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B59" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="141" t="s">
+      <c r="C59" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="D59" s="141"/>
-      <c r="E59" s="141"/>
-      <c r="F59" s="141"/>
-      <c r="G59" s="141"/>
-      <c r="H59" s="141"/>
-      <c r="I59" s="141"/>
-      <c r="J59" s="141"/>
-      <c r="K59" s="141"/>
-      <c r="L59" s="141"/>
-      <c r="M59" s="141"/>
-      <c r="N59" s="141"/>
-      <c r="O59" s="141"/>
+      <c r="D59" s="142"/>
+      <c r="E59" s="142"/>
+      <c r="F59" s="142"/>
+      <c r="G59" s="142"/>
+      <c r="H59" s="142"/>
+      <c r="I59" s="142"/>
+      <c r="J59" s="142"/>
+      <c r="K59" s="142"/>
+      <c r="L59" s="142"/>
+      <c r="M59" s="142"/>
+      <c r="N59" s="142"/>
+      <c r="O59" s="142"/>
       <c r="Q59" s="55"/>
     </row>
     <row r="60" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B60" s="116"/>
-      <c r="C60" s="143"/>
-      <c r="D60" s="144"/>
-      <c r="E60" s="144"/>
-      <c r="F60" s="144"/>
-      <c r="G60" s="144"/>
-      <c r="H60" s="144"/>
-      <c r="I60" s="144"/>
-      <c r="J60" s="144"/>
-      <c r="K60" s="144"/>
-      <c r="L60" s="144"/>
-      <c r="M60" s="144"/>
-      <c r="N60" s="144"/>
-      <c r="O60" s="145"/>
+      <c r="C60" s="136"/>
+      <c r="D60" s="137"/>
+      <c r="E60" s="137"/>
+      <c r="F60" s="137"/>
+      <c r="G60" s="137"/>
+      <c r="H60" s="137"/>
+      <c r="I60" s="137"/>
+      <c r="J60" s="137"/>
+      <c r="K60" s="137"/>
+      <c r="L60" s="137"/>
+      <c r="M60" s="137"/>
+      <c r="N60" s="137"/>
+      <c r="O60" s="138"/>
       <c r="Q60" s="55"/>
     </row>
     <row r="61" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B61" s="116"/>
-      <c r="C61" s="143"/>
-      <c r="D61" s="144"/>
-      <c r="E61" s="144"/>
-      <c r="F61" s="144"/>
-      <c r="G61" s="144"/>
-      <c r="H61" s="144"/>
-      <c r="I61" s="144"/>
-      <c r="J61" s="144"/>
-      <c r="K61" s="144"/>
-      <c r="L61" s="144"/>
-      <c r="M61" s="144"/>
-      <c r="N61" s="144"/>
-      <c r="O61" s="145"/>
+      <c r="C61" s="136"/>
+      <c r="D61" s="137"/>
+      <c r="E61" s="137"/>
+      <c r="F61" s="137"/>
+      <c r="G61" s="137"/>
+      <c r="H61" s="137"/>
+      <c r="I61" s="137"/>
+      <c r="J61" s="137"/>
+      <c r="K61" s="137"/>
+      <c r="L61" s="137"/>
+      <c r="M61" s="137"/>
+      <c r="N61" s="137"/>
+      <c r="O61" s="138"/>
       <c r="Q61" s="55"/>
     </row>
     <row r="62" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B62" s="116"/>
-      <c r="C62" s="143"/>
-      <c r="D62" s="144"/>
-      <c r="E62" s="144"/>
-      <c r="F62" s="144"/>
-      <c r="G62" s="144"/>
-      <c r="H62" s="144"/>
-      <c r="I62" s="144"/>
-      <c r="J62" s="144"/>
-      <c r="K62" s="144"/>
-      <c r="L62" s="144"/>
-      <c r="M62" s="144"/>
-      <c r="N62" s="144"/>
-      <c r="O62" s="145"/>
+      <c r="C62" s="136"/>
+      <c r="D62" s="137"/>
+      <c r="E62" s="137"/>
+      <c r="F62" s="137"/>
+      <c r="G62" s="137"/>
+      <c r="H62" s="137"/>
+      <c r="I62" s="137"/>
+      <c r="J62" s="137"/>
+      <c r="K62" s="137"/>
+      <c r="L62" s="137"/>
+      <c r="M62" s="137"/>
+      <c r="N62" s="137"/>
+      <c r="O62" s="138"/>
       <c r="Q62" s="55"/>
     </row>
     <row r="63" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="118"/>
-      <c r="C63" s="143"/>
-      <c r="D63" s="144"/>
-      <c r="E63" s="144"/>
-      <c r="F63" s="144"/>
-      <c r="G63" s="144"/>
-      <c r="H63" s="144"/>
-      <c r="I63" s="144"/>
-      <c r="J63" s="144"/>
-      <c r="K63" s="144"/>
-      <c r="L63" s="144"/>
-      <c r="M63" s="144"/>
-      <c r="N63" s="144"/>
-      <c r="O63" s="145"/>
+      <c r="C63" s="136"/>
+      <c r="D63" s="137"/>
+      <c r="E63" s="137"/>
+      <c r="F63" s="137"/>
+      <c r="G63" s="137"/>
+      <c r="H63" s="137"/>
+      <c r="I63" s="137"/>
+      <c r="J63" s="137"/>
+      <c r="K63" s="137"/>
+      <c r="L63" s="137"/>
+      <c r="M63" s="137"/>
+      <c r="N63" s="137"/>
+      <c r="O63" s="138"/>
       <c r="Q63" s="55"/>
     </row>
     <row r="64" spans="1:17" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="10"/>
       <c r="B64" s="117"/>
-      <c r="C64" s="143"/>
-      <c r="D64" s="144"/>
-      <c r="E64" s="144"/>
-      <c r="F64" s="144"/>
-      <c r="G64" s="144"/>
-      <c r="H64" s="144"/>
-      <c r="I64" s="144"/>
-      <c r="J64" s="144"/>
-      <c r="K64" s="144"/>
-      <c r="L64" s="144"/>
-      <c r="M64" s="144"/>
-      <c r="N64" s="144"/>
-      <c r="O64" s="145"/>
+      <c r="C64" s="136"/>
+      <c r="D64" s="137"/>
+      <c r="E64" s="137"/>
+      <c r="F64" s="137"/>
+      <c r="G64" s="137"/>
+      <c r="H64" s="137"/>
+      <c r="I64" s="137"/>
+      <c r="J64" s="137"/>
+      <c r="K64" s="137"/>
+      <c r="L64" s="137"/>
+      <c r="M64" s="137"/>
+      <c r="N64" s="137"/>
+      <c r="O64" s="138"/>
       <c r="Q64" s="55"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
@@ -15391,17 +15455,13 @@
     <sortCondition descending="1" ref="B60"/>
   </sortState>
   <mergeCells count="34">
-    <mergeCell ref="C60:O60"/>
-    <mergeCell ref="C61:O61"/>
-    <mergeCell ref="C62:O62"/>
-    <mergeCell ref="C63:O63"/>
-    <mergeCell ref="C64:O64"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="J29:O29"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="N2:O2"/>
     <mergeCell ref="B58:O58"/>
     <mergeCell ref="C59:O59"/>
     <mergeCell ref="B42:O42"/>
@@ -15418,13 +15478,17 @@
     <mergeCell ref="C54:O54"/>
     <mergeCell ref="C55:O55"/>
     <mergeCell ref="C56:O56"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="J29:O29"/>
+    <mergeCell ref="C60:O60"/>
+    <mergeCell ref="C61:O61"/>
+    <mergeCell ref="C62:O62"/>
+    <mergeCell ref="C63:O63"/>
+    <mergeCell ref="C64:O64"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -15433,11 +15497,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219C6488-1DAA-4551-83F9-B5C0CA1B377F}">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE676758-77EB-4B59-88DD-BEEA1E465CDA}">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15445,205 +15509,218 @@
     <col min="1" max="1" width="1.77734375" style="58" customWidth="1"/>
     <col min="2" max="2" width="3.88671875" style="58" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.6640625" style="58" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" style="58" customWidth="1"/>
     <col min="5" max="5" width="46.21875" style="58" customWidth="1"/>
-    <col min="6" max="6" width="1.77734375" style="58" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="58"/>
+    <col min="6" max="6" width="14.109375" style="58" customWidth="1"/>
+    <col min="7" max="7" width="1.77734375" style="58" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="1:6" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
-      <c r="E2" s="146" t="s">
+      <c r="E2" s="149" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F2" s="127"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="149"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="59"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="59"/>
       <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="115" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="147" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="147"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="59"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="59"/>
       <c r="B8" s="59"/>
       <c r="C8" s="115" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="147" t="s">
-        <v>27</v>
+        <v>125</v>
       </c>
       <c r="E8" s="147"/>
-      <c r="F8" s="59"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="147"/>
+      <c r="G8" s="59"/>
+    </row>
+    <row r="9" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="59"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="115" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="147" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9" s="147"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
       <c r="F9" s="59"/>
-    </row>
-    <row r="10" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="59"/>
+    </row>
+    <row r="10" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="59"/>
-      <c r="B10" s="105"/>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="59"/>
-    </row>
-    <row r="11" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="59"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="59"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="121"/>
-      <c r="F11" s="59"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="148" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="148"/>
+      <c r="D11" s="148"/>
+      <c r="E11" s="148"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="59"/>
+    </row>
+    <row r="12" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="59"/>
-      <c r="B12" s="148" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="148"/>
-      <c r="D12" s="148"/>
-      <c r="E12" s="148"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
       <c r="F12" s="59"/>
-    </row>
-    <row r="13" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="59"/>
+    </row>
+    <row r="13" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="59"/>
-      <c r="B13" s="105"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="59"/>
-    </row>
-    <row r="14" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="128"/>
+      <c r="F13" s="128"/>
+      <c r="G13" s="59"/>
+    </row>
+    <row r="14" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="59"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="121"/>
-      <c r="F14" s="59"/>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="150" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="150"/>
+      <c r="D14" s="150"/>
+      <c r="E14" s="150"/>
+      <c r="F14" s="150"/>
+      <c r="G14" s="59"/>
+    </row>
+    <row r="15" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="59"/>
-      <c r="B15" s="149" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="149"/>
-      <c r="D15" s="149"/>
-      <c r="E15" s="149"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
       <c r="F15" s="59"/>
-    </row>
-    <row r="16" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="59"/>
-      <c r="B16" s="105"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="59"/>
-    </row>
-    <row r="17" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="122"/>
-      <c r="B17" s="122"/>
-      <c r="C17" s="122"/>
-      <c r="D17" s="122"/>
+      <c r="G15" s="59"/>
+    </row>
+    <row r="16" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="121"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="122"/>
+      <c r="F16" s="122"/>
+      <c r="G16" s="121"/>
+    </row>
+    <row r="17" spans="1:7" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="121"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
       <c r="E17" s="123"/>
-      <c r="F17" s="122"/>
-    </row>
-    <row r="18" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="122"/>
+      <c r="F17" s="123"/>
+      <c r="G17" s="121"/>
+    </row>
+    <row r="18" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="121"/>
       <c r="B18" s="124"/>
       <c r="C18" s="124"/>
       <c r="D18" s="124"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="122"/>
-    </row>
-    <row r="19" spans="1:6" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="122"/>
-      <c r="B19" s="125"/>
-      <c r="C19" s="125"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="122"/>
-    </row>
-    <row r="20" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="122"/>
-      <c r="B20" s="122"/>
-      <c r="C20" s="122"/>
-      <c r="D20" s="122"/>
-      <c r="E20" s="122"/>
-      <c r="F20" s="122"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E21" s="127">
+      <c r="E18" s="125"/>
+      <c r="F18" s="125"/>
+      <c r="G18" s="121"/>
+    </row>
+    <row r="19" spans="1:7" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="121"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="121"/>
+      <c r="D19" s="121"/>
+      <c r="E19" s="121"/>
+      <c r="F19" s="121"/>
+      <c r="G19" s="121"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E20" s="126">
         <f ca="1">TODAY()</f>
-        <v>44289</v>
-      </c>
+        <v>44294</v>
+      </c>
+      <c r="F20" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B14:F14"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" xr:uid="{5A2BA084-58FD-46A3-BEB4-74D7F421E0D5}"/>
-    <hyperlink ref="D9" r:id="rId2" xr:uid="{BCDC191A-9F89-44A6-9213-D916DE8D3BF3}"/>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{874D142A-0038-42DA-A8B6-2DCDCC0CBA86}"/>
+    <hyperlink ref="D8" r:id="rId2" xr:uid="{440F480C-E2FF-4F39-9CA3-4CD48BA6AAEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -15652,6 +15729,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007CF503AC9CD2F54BA0E19C8B35D80C21" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f804e1dfc7b5d27997e3a7d590482d2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -15765,33 +15857,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7123125C-4609-4D51-BFBF-97B888D91F93}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DBF3B54-18FF-425E-9D16-518FEEB123AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15812,9 +15881,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DBF3B54-18FF-425E-9D16-518FEEB123AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7123125C-4609-4D51-BFBF-97B888D91F93}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>